<commit_message>
bo sung ki tu so
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/dataoutadac.xlsx
+++ b/app/src/main/res/raw/dataoutadac.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Android\Steno\app\src\main\res\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D7F1115-FC50-4F8C-B051-B11B9B96B4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE200BF2-7EC5-44FC-9D6B-B27363C7FCF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="911">
   <si>
     <t>a1d1</t>
   </si>
@@ -2362,9 +2362,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>c31d</t>
-  </si>
-  <si>
     <t>c3d2</t>
   </si>
   <si>
@@ -2687,6 +2684,75 @@
   </si>
   <si>
     <t>đuê</t>
+  </si>
+  <si>
+    <t>c3d1</t>
+  </si>
+  <si>
+    <t>c3d8</t>
+  </si>
+  <si>
+    <t>gị</t>
+  </si>
+  <si>
+    <t>SFTc4e6</t>
+  </si>
+  <si>
+    <t>gĩ</t>
+  </si>
+  <si>
+    <t>SFTc4e5</t>
+  </si>
+  <si>
+    <t>gỉ</t>
+  </si>
+  <si>
+    <t>SFTc4e4</t>
+  </si>
+  <si>
+    <t>gì</t>
+  </si>
+  <si>
+    <t>SFTc4e3</t>
+  </si>
+  <si>
+    <t>gí</t>
+  </si>
+  <si>
+    <t>SFTc4e2</t>
+  </si>
+  <si>
+    <t>SFTc4e1</t>
+  </si>
+  <si>
+    <t>SFTc5e8</t>
+  </si>
+  <si>
+    <t>SFTc5e7</t>
+  </si>
+  <si>
+    <t>SFTc5d8</t>
+  </si>
+  <si>
+    <t>SFTc5d7</t>
+  </si>
+  <si>
+    <t>SFTc5d6</t>
+  </si>
+  <si>
+    <t>SFTc5d5</t>
+  </si>
+  <si>
+    <t>SFTc5d4</t>
+  </si>
+  <si>
+    <t>SFTc5d3</t>
+  </si>
+  <si>
+    <t>SFTc5d2</t>
+  </si>
+  <si>
+    <t>SFTc5d1</t>
   </si>
 </sst>
 </file>
@@ -3047,10 +3113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="H1:N446"/>
+  <dimension ref="H1:N462"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="J139" sqref="J139"/>
+    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
+      <selection activeCell="K448" sqref="K448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3513,10 +3579,10 @@
     </row>
     <row r="58" spans="8:9">
       <c r="H58" t="s">
+        <v>849</v>
+      </c>
+      <c r="I58" t="s">
         <v>850</v>
-      </c>
-      <c r="I58" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="59" spans="8:9">
@@ -3620,7 +3686,7 @@
         <v>118</v>
       </c>
       <c r="I71" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="72" spans="8:9">
@@ -3721,10 +3787,10 @@
     </row>
     <row r="84" spans="8:13">
       <c r="H84" t="s">
+        <v>816</v>
+      </c>
+      <c r="I84" t="s">
         <v>817</v>
-      </c>
-      <c r="I84" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="85" spans="8:13">
@@ -3732,7 +3798,7 @@
         <v>146</v>
       </c>
       <c r="I85" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="86" spans="8:13">
@@ -3883,7 +3949,7 @@
         <v>178</v>
       </c>
       <c r="I103" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="M103" s="1"/>
     </row>
@@ -3964,7 +4030,7 @@
         <v>194</v>
       </c>
       <c r="I113" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="114" spans="8:9">
@@ -4028,7 +4094,7 @@
         <v>404</v>
       </c>
       <c r="I121" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
     </row>
     <row r="122" spans="8:9">
@@ -4124,7 +4190,7 @@
         <v>417</v>
       </c>
       <c r="I133" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="134" spans="8:9">
@@ -4153,10 +4219,10 @@
     </row>
     <row r="137" spans="8:9">
       <c r="H137" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="I137" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="138" spans="8:9">
@@ -4188,7 +4254,7 @@
         <v>551</v>
       </c>
       <c r="I141" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="142" spans="8:9">
@@ -4201,10 +4267,10 @@
     </row>
     <row r="143" spans="8:9">
       <c r="H143" t="s">
+        <v>846</v>
+      </c>
+      <c r="I143" t="s">
         <v>847</v>
-      </c>
-      <c r="I143" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="144" spans="8:9">
@@ -4228,7 +4294,7 @@
         <v>553</v>
       </c>
       <c r="I146" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="147" spans="8:9">
@@ -4324,7 +4390,7 @@
         <v>307</v>
       </c>
       <c r="I158" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="159" spans="8:9">
@@ -4484,7 +4550,7 @@
         <v>341</v>
       </c>
       <c r="I178" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="179" spans="8:9">
@@ -4548,7 +4614,7 @@
         <v>355</v>
       </c>
       <c r="I186" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="187" spans="8:9">
@@ -4612,7 +4678,7 @@
         <v>368</v>
       </c>
       <c r="I194" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="195" spans="8:9">
@@ -4676,7 +4742,7 @@
         <v>381</v>
       </c>
       <c r="I202" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="203" spans="8:9">
@@ -5225,10 +5291,10 @@
     </row>
     <row r="271" spans="8:9">
       <c r="H271" t="s">
+        <v>832</v>
+      </c>
+      <c r="I271" t="s">
         <v>833</v>
-      </c>
-      <c r="I271" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="272" spans="8:9">
@@ -5244,7 +5310,7 @@
         <v>441</v>
       </c>
       <c r="I273" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="274" spans="8:9">
@@ -5313,10 +5379,10 @@
     </row>
     <row r="282" spans="8:9">
       <c r="H282" t="s">
+        <v>830</v>
+      </c>
+      <c r="I282" t="s">
         <v>831</v>
-      </c>
-      <c r="I282" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="283" spans="8:9">
@@ -5329,10 +5395,10 @@
     </row>
     <row r="284" spans="8:9">
       <c r="H284" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="I284" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="285" spans="8:9">
@@ -5361,10 +5427,10 @@
     </row>
     <row r="288" spans="8:9">
       <c r="H288" t="s">
+        <v>818</v>
+      </c>
+      <c r="I288" t="s">
         <v>819</v>
-      </c>
-      <c r="I288" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="289" spans="8:9">
@@ -5380,7 +5446,7 @@
         <v>461</v>
       </c>
       <c r="I290" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="291" spans="8:9">
@@ -5409,18 +5475,18 @@
     </row>
     <row r="294" spans="8:9">
       <c r="H294" t="s">
+        <v>834</v>
+      </c>
+      <c r="I294" t="s">
         <v>835</v>
-      </c>
-      <c r="I294" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="295" spans="8:9">
       <c r="H295" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="I295" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="296" spans="8:9">
@@ -5444,7 +5510,7 @@
         <v>575</v>
       </c>
       <c r="I298" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="299" spans="8:9">
@@ -5468,7 +5534,7 @@
         <v>473</v>
       </c>
       <c r="I301" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="302" spans="8:9">
@@ -5492,7 +5558,7 @@
         <v>577</v>
       </c>
       <c r="I304" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="305" spans="8:14">
@@ -5556,7 +5622,7 @@
         <v>586</v>
       </c>
       <c r="I312" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="313" spans="8:14">
@@ -5588,26 +5654,26 @@
     </row>
     <row r="316" spans="8:14">
       <c r="H316" t="s">
+        <v>838</v>
+      </c>
+      <c r="I316" t="s">
         <v>839</v>
-      </c>
-      <c r="I316" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="317" spans="8:14">
       <c r="H317" t="s">
+        <v>840</v>
+      </c>
+      <c r="I317" t="s">
         <v>841</v>
-      </c>
-      <c r="I317" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="318" spans="8:14">
       <c r="H318" t="s">
+        <v>842</v>
+      </c>
+      <c r="I318" t="s">
         <v>843</v>
-      </c>
-      <c r="I318" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="319" spans="8:14">
@@ -5620,58 +5686,58 @@
     </row>
     <row r="320" spans="8:14">
       <c r="H320" t="s">
-        <v>780</v>
+        <v>888</v>
       </c>
       <c r="I320" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="321" spans="8:9">
       <c r="H321" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="I321" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="322" spans="8:9">
       <c r="H322" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="I322" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="323" spans="8:9">
       <c r="H323" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I323" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="324" spans="8:9">
       <c r="H324" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="I324" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="325" spans="8:9">
       <c r="H325" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="I325" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="326" spans="8:9">
       <c r="H326" t="s">
-        <v>785</v>
+        <v>889</v>
       </c>
       <c r="I326" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="327" spans="8:9">
@@ -6020,26 +6086,26 @@
     </row>
     <row r="370" spans="8:9">
       <c r="H370" t="s">
+        <v>857</v>
+      </c>
+      <c r="I370" t="s">
         <v>858</v>
-      </c>
-      <c r="I370" t="s">
-        <v>859</v>
       </c>
     </row>
     <row r="371" spans="8:9">
       <c r="H371" t="s">
+        <v>859</v>
+      </c>
+      <c r="I371" t="s">
         <v>860</v>
-      </c>
-      <c r="I371" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="372" spans="8:9">
       <c r="H372" t="s">
+        <v>881</v>
+      </c>
+      <c r="I372" t="s">
         <v>882</v>
-      </c>
-      <c r="I372" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="373" spans="8:9">
@@ -6052,66 +6118,66 @@
     </row>
     <row r="374" spans="8:9">
       <c r="H374" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="I374" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="375" spans="8:9">
       <c r="H375" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I375" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="376" spans="8:9">
       <c r="H376" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="I376" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="377" spans="8:9">
       <c r="H377" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="I377" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="378" spans="8:9">
       <c r="H378" t="s">
+        <v>862</v>
+      </c>
+      <c r="I378" t="s">
         <v>863</v>
-      </c>
-      <c r="I378" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="379" spans="8:9">
       <c r="H379" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="I379" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
     </row>
     <row r="380" spans="8:9">
       <c r="H380" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="I380" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="381" spans="8:9">
       <c r="H381" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="I381" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="382" spans="8:9">
@@ -6132,18 +6198,18 @@
     </row>
     <row r="384" spans="8:9">
       <c r="H384" t="s">
+        <v>824</v>
+      </c>
+      <c r="I384" t="s">
         <v>825</v>
-      </c>
-      <c r="I384" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="385" spans="8:9">
       <c r="H385" t="s">
+        <v>826</v>
+      </c>
+      <c r="I385" t="s">
         <v>827</v>
-      </c>
-      <c r="I385" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="386" spans="8:9">
@@ -6207,7 +6273,7 @@
         <v>650</v>
       </c>
       <c r="I393" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="394" spans="8:9">
@@ -6380,18 +6446,18 @@
     </row>
     <row r="415" spans="8:9">
       <c r="H415" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="I415" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="416" spans="8:9">
       <c r="H416" t="s">
+        <v>822</v>
+      </c>
+      <c r="I416" t="s">
         <v>823</v>
-      </c>
-      <c r="I416" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="417" spans="8:9">
@@ -6420,10 +6486,10 @@
     </row>
     <row r="420" spans="8:9">
       <c r="H420" t="s">
+        <v>883</v>
+      </c>
+      <c r="I420" t="s">
         <v>884</v>
-      </c>
-      <c r="I420" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="421" spans="8:9">
@@ -6444,58 +6510,58 @@
     </row>
     <row r="423" spans="8:9">
       <c r="H423" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="I423" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="424" spans="8:9">
       <c r="H424" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="I424" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="425" spans="8:9">
       <c r="H425" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="I425" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="426" spans="8:9">
       <c r="H426" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="I426" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="427" spans="8:9">
       <c r="H427" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="I427" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="428" spans="8:9">
       <c r="H428" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="I428" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="429" spans="8:9">
       <c r="H429" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="I429" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="430" spans="8:9">
@@ -6527,7 +6593,7 @@
         <v>695</v>
       </c>
       <c r="I433" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="434" spans="8:9">
@@ -6556,10 +6622,10 @@
     </row>
     <row r="437" spans="8:9">
       <c r="H437" t="s">
+        <v>886</v>
+      </c>
+      <c r="I437" t="s">
         <v>887</v>
-      </c>
-      <c r="I437" t="s">
-        <v>888</v>
       </c>
     </row>
     <row r="438" spans="8:9">
@@ -6580,10 +6646,10 @@
     </row>
     <row r="440" spans="8:9">
       <c r="H440" t="s">
+        <v>820</v>
+      </c>
+      <c r="I440" t="s">
         <v>821</v>
-      </c>
-      <c r="I440" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="441" spans="8:9">
@@ -6632,6 +6698,134 @@
       </c>
       <c r="I446" t="s">
         <v>760</v>
+      </c>
+    </row>
+    <row r="447" spans="8:9">
+      <c r="H447" t="s">
+        <v>910</v>
+      </c>
+      <c r="I447">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="448" spans="8:9">
+      <c r="H448" t="s">
+        <v>909</v>
+      </c>
+      <c r="I448">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="449" spans="8:9">
+      <c r="H449" t="s">
+        <v>908</v>
+      </c>
+      <c r="I449">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="450" spans="8:9">
+      <c r="H450" t="s">
+        <v>907</v>
+      </c>
+      <c r="I450">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="451" spans="8:9">
+      <c r="H451" t="s">
+        <v>906</v>
+      </c>
+      <c r="I451">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="452" spans="8:9">
+      <c r="H452" t="s">
+        <v>905</v>
+      </c>
+      <c r="I452">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="453" spans="8:9">
+      <c r="H453" t="s">
+        <v>904</v>
+      </c>
+      <c r="I453">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="454" spans="8:9">
+      <c r="H454" t="s">
+        <v>903</v>
+      </c>
+      <c r="I454">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="455" spans="8:9">
+      <c r="H455" t="s">
+        <v>902</v>
+      </c>
+      <c r="I455">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456" spans="8:9">
+      <c r="H456" t="s">
+        <v>901</v>
+      </c>
+      <c r="I456">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="457" spans="8:9">
+      <c r="H457" t="s">
+        <v>900</v>
+      </c>
+      <c r="I457" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="458" spans="8:9">
+      <c r="H458" t="s">
+        <v>899</v>
+      </c>
+      <c r="I458" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="459" spans="8:9">
+      <c r="H459" t="s">
+        <v>897</v>
+      </c>
+      <c r="I459" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="460" spans="8:9">
+      <c r="H460" t="s">
+        <v>895</v>
+      </c>
+      <c r="I460" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="461" spans="8:9">
+      <c r="H461" t="s">
+        <v>893</v>
+      </c>
+      <c r="I461" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="462" spans="8:9">
+      <c r="H462" t="s">
+        <v>891</v>
+      </c>
+      <c r="I462" t="s">
+        <v>890</v>
       </c>
     </row>
   </sheetData>

</xml_diff>